<commit_message>
added top sector %NAV in excel and AgGrid
</commit_message>
<xml_diff>
--- a/static/JPMorgan_5-ETF-extract.xlsx
+++ b/static/JPMorgan_5-ETF-extract.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\ETF-Dashboard\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102FBB00-4353-4A1F-9BCB-9601BACB6210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7248A4D1-51DD-4348-94C5-39E48374ECFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{480BDBAF-5390-49AF-AD03-EFAB7C68E97F}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{480BDBAF-5390-49AF-AD03-EFAB7C68E97F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t>Fund Actively Managed</t>
   </si>
@@ -168,6 +168,54 @@
   </si>
   <si>
     <t>JQUA US Equity</t>
+  </si>
+  <si>
+    <t>Top 5 Sector</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top 5 %NAV</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Technology,Health Care,Industrials,Consumer Staples,Financials</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>17.7,12.0,12.0,11.1,7.1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Financials,Consumer Discretionary,Government,Industrials,Technology</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>31.5,5.3,2.3,1.79,1.62</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Financials,Health Care,Consumer Staples,Consumer Discretionary,Technology</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.1,12.7,11.2,10.6,9.9</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Technology,Communications,Consumer Discretionary,Health Care,Consumer Staples</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>41.5,14.4,10.8,5.8,5.4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Technology,Health Care,Consumer Discretionary,Communications,Consumer Staples</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>35.2,13.4,10.4,7.9,6.3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -583,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAC6CD23-7E11-4BD7-A137-D6260AD51D15}">
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="P4" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -653,14 +701,18 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
+      <c r="U1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" ht="93.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -721,14 +773,18 @@
       <c r="T2" s="4">
         <v>0.629</v>
       </c>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
+      <c r="U2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" ht="93.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -787,14 +843,18 @@
       <c r="T3" s="4">
         <v>0.94799999999999995</v>
       </c>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
+      <c r="U3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="120" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -847,14 +907,18 @@
         <v>1.095</v>
       </c>
       <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
+      <c r="U4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:26" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" ht="120" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -907,14 +971,18 @@
         <v>0.63200000000000001</v>
       </c>
       <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
+      <c r="U5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:26" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="120" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
@@ -975,8 +1043,12 @@
       <c r="T6" s="4">
         <v>0.997</v>
       </c>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
+      <c r="U6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>

</xml_diff>

<commit_message>
added BBIN US Equity to Excel
</commit_message>
<xml_diff>
--- a/static/JPMorgan_5-ETF-extract.xlsx
+++ b/static/JPMorgan_5-ETF-extract.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\ETF-Dashboard\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7248A4D1-51DD-4348-94C5-39E48374ECFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7F0B0E-395C-407E-A73D-36EA8E697FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{480BDBAF-5390-49AF-AD03-EFAB7C68E97F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{480BDBAF-5390-49AF-AD03-EFAB7C68E97F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
   <si>
     <t>Fund Actively Managed</t>
   </si>
@@ -215,6 +215,23 @@
   </si>
   <si>
     <t>35.2,13.4,10.4,7.9,6.3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPM BETABUILDERS INTL EQTY</t>
+  </si>
+  <si>
+    <t>Cboe BZX Exchange (Cboe BZX)</t>
+  </si>
+  <si>
+    <t>BBIN US Equity</t>
+  </si>
+  <si>
+    <t>Financials,Industrials,Health Care,Consumer Staples,Consumer Discretionary</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>18.8,13.8,13.0,11.0,10.7</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -629,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAC6CD23-7E11-4BD7-A137-D6260AD51D15}">
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P4" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" topLeftCell="R5" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1054,6 +1071,78 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
+    <row r="7" spans="1:26" ht="120" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3706.97</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L7" s="4">
+        <v>3.4289999999999998</v>
+      </c>
+      <c r="M7" s="4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="N7" s="4">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="O7" s="4">
+        <v>22.239000000000001</v>
+      </c>
+      <c r="P7" s="4">
+        <v>19.305</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="R7" s="4">
+        <v>0.315</v>
+      </c>
+      <c r="S7" s="4">
+        <v>1.099</v>
+      </c>
+      <c r="T7" s="4">
+        <v>1.0189999999999999</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>